<commit_message>
Ajustes para permitir cadastro sem email
</commit_message>
<xml_diff>
--- a/1 - WebApi/Cipa.WebApi/Assets/Template Importacao.xlsx
+++ b/1 - WebApi/Cipa.WebApi/Assets/Template Importacao.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t xml:space="preserve">Matrícula</t>
   </si>
@@ -56,34 +56,15 @@
   </si>
   <si>
     <t xml:space="preserve">E-mail do Gestor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jose@email.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">José</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Teste</t>
-  </si>
-  <si>
-    <t xml:space="preserve">usuariorede</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Testando 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="d/m/yyyy"/>
-    <numFmt numFmtId="166" formatCode="dd/mm/yy"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -164,7 +145,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -178,10 +159,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -202,13 +179,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="1" style="1" width="19.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="19.89"/>
@@ -250,60 +227,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
-        <v>22222</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="4" t="n">
-        <v>43871</v>
-      </c>
-      <c r="I2" s="4" t="n">
-        <v>35114</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
-        <v>33333</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I3" s="4"/>
-    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B2:B1003" type="list">
+    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B2:B1001" type="list">
       <formula1>"Usuário de Rede,E-mail"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="jose@email.com"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>